<commit_message>
created falling, struggle and walkingToRunning classes to dataset and ran on minirocket using 10 fold cross validation to get a confusion matrix and accuracy
</commit_message>
<xml_diff>
--- a/spliced/falling/2023-03-21_15-34-04/accelerometer_selected.xlsx
+++ b/spliced/falling/2023-03-21_15-34-04/accelerometer_selected.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -670,17 +670,6 @@
         <v>0.7879237532615664</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>-0.4122457504272466</v>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.09671294689178367</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.6507992744445799</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding the changes we made on may 9th
</commit_message>
<xml_diff>
--- a/spliced/falling/2023-03-21_15-34-04/accelerometer_selected.xlsx
+++ b/spliced/falling/2023-03-21_15-34-04/accelerometer_selected.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,222 +452,332 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.4068026542663569</v>
+        <v>-0.772541880607605</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.1559689044952389</v>
+        <v>-0.2669219076633453</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6923939287662497</v>
+        <v>0.974086582660675</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.133467555046082</v>
+        <v>-0.4068026542663569</v>
       </c>
       <c r="B3" t="n">
-        <v>0.02078273892402592</v>
+        <v>-0.1559689044952389</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06124181300401743</v>
+        <v>0.6923939287662497</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.8061990737915055</v>
+        <v>-0.133467555046082</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.673800706863404</v>
+        <v>0.02078273892402592</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9037782549858108</v>
+        <v>0.06124181300401743</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-2.158628642559052</v>
+        <v>-0.8061990737915055</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.300643742084504</v>
+        <v>-0.673800706863404</v>
       </c>
       <c r="C5" t="n">
-        <v>2.320873700082303</v>
+        <v>0.9037782549858108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-5.611039400100712</v>
+        <v>-2.158628642559052</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.067752599716186</v>
+        <v>-1.300643742084504</v>
       </c>
       <c r="C6" t="n">
-        <v>3.571036458015443</v>
+        <v>2.320873700082303</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>10.29619103670124</v>
+        <v>-5.611039400100712</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.212279349565506</v>
+        <v>-1.067752599716186</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.306954741477978</v>
+        <v>3.571036458015443</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>16.49048757553099</v>
+        <v>10.29619103670124</v>
       </c>
       <c r="B8" t="n">
-        <v>-2.535040378570561</v>
+        <v>-1.212279349565506</v>
       </c>
       <c r="C8" t="n">
-        <v>-4.817432403564455</v>
+        <v>-1.306954741477978</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5.932503581047048</v>
+        <v>16.49048757553099</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.061056911945345</v>
+        <v>-2.535040378570561</v>
       </c>
       <c r="C9" t="n">
-        <v>-3.269190549850461</v>
+        <v>-4.817432403564455</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-3.17936980724334</v>
+        <v>5.932503581047048</v>
       </c>
       <c r="B10" t="n">
-        <v>-6.029928088188166</v>
+        <v>-5.061056911945345</v>
       </c>
       <c r="C10" t="n">
-        <v>1.175602436065679</v>
+        <v>-3.269190549850461</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.0117866396904</v>
+        <v>-3.17936980724334</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.052042245864868</v>
+        <v>-6.029928088188166</v>
       </c>
       <c r="C11" t="n">
-        <v>4.367893397808076</v>
+        <v>1.175602436065679</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.2356891632080053</v>
+        <v>2.0117866396904</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.266632080078124</v>
+        <v>-2.052042245864868</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6566014289855999</v>
+        <v>4.367893397808076</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-0.9150051474571261</v>
+        <v>0.2356891632080053</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.8746488094329823</v>
+        <v>-1.266632080078124</v>
       </c>
       <c r="C13" t="n">
-        <v>2.565791487693792</v>
+        <v>0.6566014289855999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-1.240249633789063</v>
+        <v>-0.9150051474571261</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.217294335365296</v>
+        <v>-0.8746488094329823</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8477112054824805</v>
+        <v>2.565791487693792</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-0.5955665111541733</v>
+        <v>-1.240249633789063</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.5654221177101116</v>
+        <v>-1.217294335365296</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.02790260314941459</v>
+        <v>0.8477112054824805</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.5104980468750013</v>
+        <v>-0.5955665111541733</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.1675477027893068</v>
+        <v>-0.5654221177101116</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.5091485977172858</v>
+        <v>-0.02790260314941459</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.036981225013732</v>
+        <v>0.5104980468750013</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.10504525899887</v>
+        <v>-0.1675477027893068</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.4656781554222081</v>
+        <v>-0.5091485977172858</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.4670617580413783</v>
+        <v>1.036981225013732</v>
       </c>
       <c r="B18" t="n">
-        <v>0.04750466346740631</v>
+        <v>-0.10504525899887</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1018033027648915</v>
+        <v>-0.4656781554222081</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-0.5187106132507345</v>
+        <v>0.4670617580413783</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.1585329174995418</v>
+        <v>0.04750466346740631</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.09741693735122439</v>
+        <v>0.1018033027648915</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-1.071794033050533</v>
+        <v>-0.5187106132507345</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.06254482269287452</v>
+        <v>-0.1585329174995418</v>
       </c>
       <c r="C20" t="n">
-        <v>0.503868103027345</v>
+        <v>-0.09741693735122439</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
+        <v>-1.071794033050533</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.06254482269287452</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.503868103027345</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>-0.1770309805870052</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B22" t="n">
         <v>-0.8330835700035099</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C22" t="n">
         <v>0.7879237532615664</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>-0.4122457504272466</v>
+      </c>
+      <c r="B23" t="n">
+        <v>-0.09671294689178367</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.6507992744445799</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>-0.01871716976165649</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.1319747567176817</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-0.1633049249649066</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>-0.1193938255310074</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-0.05726575851440492</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-0.4602591991424554</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>-0.2904316186904892</v>
+      </c>
+      <c r="B26" t="n">
+        <v>-0.1059370636939995</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.1864967942237846</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.0775488615036011</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-0.0401190519332886</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.02606511116027833</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>-0.02678942680358923</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-0.3534234166145316</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-0.111013770103454</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>-0.1420207023620607</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-0.1315011978149412</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.04810285568237234</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>-0.1982678174972537</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-0.0857929587364194</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-0.1000801920890816</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.08944976329803658</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.1226030588150037</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-0.6240378618240389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>